<commit_message>
Updated documentation. Cleaned up a bit.
</commit_message>
<xml_diff>
--- a/CSVs/Table1.xlsx
+++ b/CSVs/Table1.xlsx
@@ -40,21 +40,21 @@
     <t>score</t>
   </si>
   <si>
+    <t>typical_sleep_duration</t>
+  </si>
+  <si>
+    <t>age_at_test</t>
+  </si>
+  <si>
     <t>np.power(typical_sleep_duration, 2)</t>
   </si>
   <si>
-    <t>age_at_test</t>
-  </si>
-  <si>
-    <t>typical_sleep_duration</t>
+    <t>age_at_test:np.power(typical_sleep_duration, 2)</t>
   </si>
   <si>
     <t>age_at_test:typical_sleep_duration</t>
   </si>
   <si>
-    <t>age_at_test:np.power(typical_sleep_duration, 2)</t>
-  </si>
-  <si>
     <t>STM</t>
   </si>
   <si>
@@ -67,6 +67,18 @@
     <t>Overall</t>
   </si>
   <si>
+    <t xml:space="preserve">    0.0177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.0302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.0357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.0445</t>
+  </si>
+  <si>
     <t xml:space="preserve">   -0.0048</t>
   </si>
   <si>
@@ -79,18 +91,6 @@
     <t xml:space="preserve">   -0.0230</t>
   </si>
   <si>
-    <t xml:space="preserve">    0.0177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.0302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.0357</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.0445</t>
-  </si>
-  <si>
     <t xml:space="preserve">   -0.0254</t>
   </si>
   <si>
@@ -103,9 +103,18 @@
     <t xml:space="preserve">   -0.0334</t>
   </si>
   <si>
+    <t xml:space="preserve">    0.0003</t>
+  </si>
+  <si>
     <t xml:space="preserve">    0.0002</t>
   </si>
   <si>
+    <t xml:space="preserve">   -0.0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.0001</t>
+  </si>
+  <si>
     <t xml:space="preserve">   -0.0002</t>
   </si>
   <si>
@@ -115,13 +124,10 @@
     <t>-3.147e-05</t>
   </si>
   <si>
-    <t xml:space="preserve">    0.0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -0.0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.0001</t>
+    <t xml:space="preserve">    0.007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.008</t>
   </si>
   <si>
     <t xml:space="preserve">    0.003</t>
@@ -130,18 +136,24 @@
     <t xml:space="preserve">    0.004</t>
   </si>
   <si>
-    <t xml:space="preserve">    0.007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.008</t>
-  </si>
-  <si>
     <t xml:space="preserve">    0.001</t>
   </si>
   <si>
     <t xml:space="preserve">    0.000</t>
   </si>
   <si>
+    <t xml:space="preserve">    2.394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6.341</t>
+  </si>
+  <si>
     <t xml:space="preserve">   -1.425</t>
   </si>
   <si>
@@ -154,18 +166,6 @@
     <t xml:space="preserve">   -7.170</t>
   </si>
   <si>
-    <t xml:space="preserve">    2.394</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    4.194</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    4.460</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    6.341</t>
-  </si>
-  <si>
     <t xml:space="preserve">  -34.757</t>
   </si>
   <si>
@@ -178,6 +178,18 @@
     <t xml:space="preserve">  -48.098</t>
   </si>
   <si>
+    <t xml:space="preserve">    1.199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1.447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.733</t>
+  </si>
+  <si>
     <t xml:space="preserve">    0.343</t>
   </si>
   <si>
@@ -190,25 +202,25 @@
     <t xml:space="preserve">   -0.068</t>
   </si>
   <si>
-    <t xml:space="preserve">    1.199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    1.053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -1.447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.733</t>
+    <t xml:space="preserve"> 0.017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.000</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.154</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.017</t>
+    <t xml:space="preserve"> 0.231</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.292</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.148</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.464</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.732</t>
@@ -223,16 +235,13 @@
     <t xml:space="preserve"> 0.945</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.231</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.292</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.148</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.464</t>
+    <t xml:space="preserve">    0.016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.031</t>
   </si>
   <si>
     <t xml:space="preserve">   -0.011</t>
@@ -247,15 +256,6 @@
     <t xml:space="preserve">   -0.029</t>
   </si>
   <si>
-    <t xml:space="preserve">    0.016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.031</t>
-  </si>
-  <si>
     <t xml:space="preserve">   -0.027</t>
   </si>
   <si>
@@ -265,10 +265,22 @@
     <t xml:space="preserve">   -0.035</t>
   </si>
   <si>
+    <t xml:space="preserve">   -0.000</t>
+  </si>
+  <si>
     <t xml:space="preserve">   -0.001</t>
   </si>
   <si>
-    <t xml:space="preserve">   -0.000</t>
+    <t xml:space="preserve">    0.032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.058</t>
   </si>
   <si>
     <t xml:space="preserve">    0.002</t>
@@ -278,18 +290,6 @@
   </si>
   <si>
     <t xml:space="preserve">   -0.017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.058</t>
   </si>
   <si>
     <t xml:space="preserve">   -0.021</t>
@@ -705,7 +705,7 @@
         <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
         <v>85</v>
@@ -729,10 +729,10 @@
         <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -753,10 +753,10 @@
         <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -777,10 +777,10 @@
         <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -803,10 +803,10 @@
         <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -830,7 +830,7 @@
         <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -904,7 +904,7 @@
         <v>80</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -925,7 +925,7 @@
         <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
         <v>92</v>
@@ -952,7 +952,7 @@
         <v>81</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1038,7 +1038,7 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
         <v>56</v>
@@ -1047,10 +1047,10 @@
         <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1085,7 +1085,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>41</v>
@@ -1109,7 +1109,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
@@ -1136,7 +1136,7 @@
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s">
         <v>60</v>
@@ -1145,10 +1145,10 @@
         <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:8">

</xml_diff>